<commit_message>
updated for alarm summary
</commit_message>
<xml_diff>
--- a/Alarm_Summary_Fire_System_PLC_1.xlsx
+++ b/Alarm_Summary_Fire_System_PLC_1.xlsx
@@ -104,7 +104,7 @@
       <sz val="8"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -123,8 +123,14 @@
         <bgColor indexed="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C0C0C0"/>
+        <bgColor rgb="00C0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -623,7 +629,76 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border/>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
@@ -631,7 +706,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -903,56 +978,78 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1370,7 +1467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="19" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
@@ -1867,933 +1964,1338 @@
       <c r="N18" s="81" t="n"/>
     </row>
     <row r="19" ht="30" customFormat="1" customHeight="1" s="1" thickBot="1">
-      <c r="A19" s="16" t="inlineStr">
+      <c r="A19" s="93" t="inlineStr">
         <is>
           <t>Tag No</t>
         </is>
       </c>
-      <c r="B19" s="17" t="inlineStr">
+      <c r="B19" s="93" t="inlineStr">
         <is>
           <t>P &amp; ID</t>
         </is>
       </c>
-      <c r="C19" s="33" t="inlineStr">
+      <c r="C19" s="94" t="inlineStr">
         <is>
           <t>Service Description</t>
         </is>
       </c>
-      <c r="D19" s="33" t="inlineStr">
+      <c r="D19" s="94" t="inlineStr">
         <is>
           <t>Range</t>
         </is>
       </c>
-      <c r="E19" s="64" t="inlineStr">
+      <c r="E19" s="94" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
       </c>
-      <c r="F19" s="18" t="inlineStr">
+      <c r="F19" s="95" t="inlineStr">
         <is>
           <t>Normal Operating
 Conditions</t>
         </is>
       </c>
-      <c r="G19" s="19" t="inlineStr">
+      <c r="G19" s="96" t="inlineStr">
         <is>
           <t>HH</t>
         </is>
       </c>
-      <c r="H19" s="20" t="inlineStr">
+      <c r="H19" s="96" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="I19" s="20" t="inlineStr">
+      <c r="I19" s="96" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
-      <c r="J19" s="21" t="inlineStr">
+      <c r="J19" s="96" t="inlineStr">
         <is>
           <t>LL</t>
         </is>
       </c>
-      <c r="K19" s="33" t="inlineStr">
+      <c r="K19" s="97" t="inlineStr">
         <is>
           <t>Engineering Notes</t>
         </is>
       </c>
-      <c r="L19" s="93" t="n"/>
-      <c r="M19" s="93" t="n"/>
-      <c r="N19" s="82" t="n"/>
+      <c r="L19" s="98" t="n"/>
+      <c r="M19" s="99" t="n"/>
+      <c r="N19" s="100" t="n"/>
+      <c r="O19" s="101" t="n"/>
+      <c r="P19" s="101" t="n"/>
+      <c r="Q19" s="101" t="n"/>
+      <c r="R19" s="101" t="n"/>
+      <c r="S19" s="101" t="n"/>
     </row>
     <row r="20" ht="15" customFormat="1" customHeight="1" s="1">
-      <c r="A20" s="94" t="inlineStr">
+      <c r="A20" s="102" t="inlineStr">
         <is>
           <t>B3:0/0</t>
         </is>
       </c>
-      <c r="B20" s="94" t="inlineStr"/>
-      <c r="C20" s="95" t="inlineStr">
+      <c r="B20" s="102" t="inlineStr"/>
+      <c r="C20" s="102" t="inlineStr">
         <is>
           <t>Fire Alarm Zone 1</t>
         </is>
       </c>
-      <c r="D20" s="96" t="inlineStr"/>
-      <c r="E20" s="97" t="inlineStr"/>
-      <c r="F20" s="98" t="inlineStr"/>
-      <c r="G20" s="99" t="inlineStr"/>
-      <c r="H20" s="100" t="inlineStr"/>
-      <c r="I20" s="100" t="inlineStr"/>
-      <c r="J20" s="100" t="inlineStr"/>
-      <c r="K20" s="101" t="inlineStr"/>
-      <c r="N20" s="82" t="n"/>
+      <c r="D20" s="103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" s="104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" s="105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" s="106" t="inlineStr"/>
+      <c r="H20" s="106" t="inlineStr"/>
+      <c r="I20" s="106" t="inlineStr"/>
+      <c r="J20" s="106" t="inlineStr"/>
+      <c r="K20" s="104" t="inlineStr"/>
+      <c r="L20" s="107" t="n"/>
+      <c r="M20" s="108" t="n"/>
+      <c r="N20" s="100" t="n"/>
+      <c r="O20" s="101" t="n"/>
+      <c r="P20" s="101" t="n"/>
+      <c r="Q20" s="101" t="n"/>
+      <c r="R20" s="101" t="n"/>
+      <c r="S20" s="101" t="n"/>
     </row>
     <row r="21" ht="15" customFormat="1" customHeight="1" s="1">
-      <c r="A21" s="102" t="inlineStr">
+      <c r="A21" s="109" t="inlineStr">
         <is>
           <t>B3:0/11</t>
         </is>
       </c>
-      <c r="B21" s="102" t="inlineStr"/>
-      <c r="C21" s="103" t="inlineStr">
+      <c r="B21" s="109" t="inlineStr"/>
+      <c r="C21" s="109" t="inlineStr">
         <is>
           <t>Fire Alarm Zone 2</t>
         </is>
       </c>
-      <c r="D21" s="104" t="inlineStr"/>
-      <c r="E21" s="105" t="inlineStr"/>
-      <c r="F21" s="102" t="inlineStr"/>
-      <c r="G21" s="100" t="inlineStr"/>
-      <c r="H21" s="100" t="inlineStr"/>
-      <c r="I21" s="100" t="inlineStr"/>
-      <c r="J21" s="100" t="inlineStr"/>
-      <c r="K21" s="101" t="inlineStr"/>
-      <c r="L21" s="57" t="n"/>
-      <c r="M21" s="57" t="n"/>
-      <c r="N21" s="82" t="n"/>
+      <c r="D21" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" s="106" t="inlineStr"/>
+      <c r="H21" s="106" t="inlineStr"/>
+      <c r="I21" s="106" t="inlineStr"/>
+      <c r="J21" s="106" t="inlineStr"/>
+      <c r="K21" s="104" t="inlineStr"/>
+      <c r="L21" s="107" t="n"/>
+      <c r="M21" s="108" t="n"/>
+      <c r="N21" s="100" t="n"/>
+      <c r="O21" s="101" t="n"/>
+      <c r="P21" s="101" t="n"/>
+      <c r="Q21" s="101" t="n"/>
+      <c r="R21" s="101" t="n"/>
+      <c r="S21" s="101" t="n"/>
     </row>
     <row r="22" ht="15" customHeight="1">
-      <c r="A22" s="102" t="inlineStr">
+      <c r="A22" s="109" t="inlineStr">
         <is>
           <t>B3:3/8</t>
         </is>
       </c>
-      <c r="B22" s="102" t="inlineStr"/>
-      <c r="C22" s="103" t="inlineStr">
+      <c r="B22" s="109" t="inlineStr"/>
+      <c r="C22" s="109" t="inlineStr">
         <is>
           <t>FE 1 Failure Alarm</t>
         </is>
       </c>
-      <c r="D22" s="104" t="inlineStr"/>
-      <c r="E22" s="105" t="inlineStr"/>
-      <c r="F22" s="106" t="inlineStr"/>
-      <c r="G22" s="107" t="inlineStr"/>
-      <c r="H22" s="108" t="inlineStr"/>
-      <c r="I22" s="109" t="inlineStr"/>
-      <c r="J22" s="108" t="inlineStr"/>
+      <c r="D22" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" s="112" t="inlineStr"/>
+      <c r="H22" s="112" t="inlineStr"/>
+      <c r="I22" s="113" t="inlineStr"/>
+      <c r="J22" s="112" t="inlineStr"/>
       <c r="K22" s="110" t="inlineStr"/>
-      <c r="N22" s="81" t="n"/>
+      <c r="L22" s="107" t="n"/>
+      <c r="M22" s="108" t="n"/>
+      <c r="N22" s="114" t="n"/>
+      <c r="O22" s="101" t="n"/>
+      <c r="P22" s="101" t="n"/>
+      <c r="Q22" s="101" t="n"/>
+      <c r="R22" s="101" t="n"/>
+      <c r="S22" s="101" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1">
-      <c r="A23" s="102" t="inlineStr">
+      <c r="A23" s="109" t="inlineStr">
         <is>
           <t>B3:3/9</t>
         </is>
       </c>
-      <c r="B23" s="102" t="inlineStr"/>
-      <c r="C23" s="103" t="inlineStr">
+      <c r="B23" s="109" t="inlineStr"/>
+      <c r="C23" s="109" t="inlineStr">
         <is>
           <t>FE 2 Failure Alarm</t>
         </is>
       </c>
-      <c r="D23" s="104" t="inlineStr"/>
-      <c r="E23" s="105" t="inlineStr"/>
-      <c r="F23" s="106" t="inlineStr"/>
-      <c r="G23" s="107" t="inlineStr"/>
-      <c r="H23" s="108" t="inlineStr"/>
-      <c r="I23" s="109" t="inlineStr"/>
-      <c r="J23" s="108" t="inlineStr"/>
+      <c r="D23" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" s="112" t="inlineStr"/>
+      <c r="H23" s="112" t="inlineStr"/>
+      <c r="I23" s="113" t="inlineStr"/>
+      <c r="J23" s="112" t="inlineStr"/>
       <c r="K23" s="110" t="inlineStr"/>
-      <c r="L23" s="63" t="n"/>
-      <c r="M23" s="63" t="n"/>
-      <c r="N23" s="81" t="n"/>
+      <c r="L23" s="107" t="n"/>
+      <c r="M23" s="108" t="n"/>
+      <c r="N23" s="114" t="n"/>
+      <c r="O23" s="101" t="n"/>
+      <c r="P23" s="101" t="n"/>
+      <c r="Q23" s="101" t="n"/>
+      <c r="R23" s="101" t="n"/>
+      <c r="S23" s="101" t="n"/>
     </row>
     <row r="24" ht="15" customHeight="1">
-      <c r="A24" s="102" t="inlineStr">
+      <c r="A24" s="109" t="inlineStr">
         <is>
           <t>B3:3/10</t>
         </is>
       </c>
-      <c r="B24" s="102" t="inlineStr"/>
-      <c r="C24" s="103" t="inlineStr">
+      <c r="B24" s="109" t="inlineStr"/>
+      <c r="C24" s="109" t="inlineStr">
         <is>
           <t>FE 3 Failure Alarm</t>
         </is>
       </c>
-      <c r="D24" s="104" t="inlineStr"/>
-      <c r="E24" s="105" t="inlineStr"/>
-      <c r="F24" s="106" t="inlineStr"/>
-      <c r="G24" s="107" t="inlineStr"/>
-      <c r="H24" s="108" t="inlineStr"/>
-      <c r="I24" s="109" t="inlineStr"/>
-      <c r="J24" s="108" t="inlineStr"/>
+      <c r="D24" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" s="112" t="inlineStr"/>
+      <c r="H24" s="112" t="inlineStr"/>
+      <c r="I24" s="113" t="inlineStr"/>
+      <c r="J24" s="112" t="inlineStr"/>
       <c r="K24" s="110" t="inlineStr"/>
-      <c r="L24" s="63" t="n"/>
-      <c r="M24" s="63" t="n"/>
-      <c r="N24" s="81" t="n"/>
+      <c r="L24" s="107" t="n"/>
+      <c r="M24" s="108" t="n"/>
+      <c r="N24" s="114" t="n"/>
+      <c r="O24" s="101" t="n"/>
+      <c r="P24" s="101" t="n"/>
+      <c r="Q24" s="101" t="n"/>
+      <c r="R24" s="101" t="n"/>
+      <c r="S24" s="101" t="n"/>
     </row>
     <row r="25" ht="15" customHeight="1">
-      <c r="A25" s="102" t="inlineStr">
+      <c r="A25" s="109" t="inlineStr">
         <is>
           <t>B3:3/11</t>
         </is>
       </c>
-      <c r="B25" s="102" t="inlineStr"/>
-      <c r="C25" s="103" t="inlineStr">
+      <c r="B25" s="109" t="inlineStr"/>
+      <c r="C25" s="109" t="inlineStr">
         <is>
           <t>FE 4 Failure Alarm</t>
         </is>
       </c>
-      <c r="D25" s="104" t="inlineStr"/>
-      <c r="E25" s="105" t="inlineStr"/>
-      <c r="F25" s="106" t="inlineStr"/>
-      <c r="G25" s="107" t="inlineStr"/>
-      <c r="H25" s="108" t="inlineStr"/>
-      <c r="I25" s="109" t="inlineStr"/>
-      <c r="J25" s="108" t="inlineStr"/>
+      <c r="D25" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" s="112" t="inlineStr"/>
+      <c r="H25" s="112" t="inlineStr"/>
+      <c r="I25" s="113" t="inlineStr"/>
+      <c r="J25" s="112" t="inlineStr"/>
       <c r="K25" s="110" t="inlineStr"/>
-      <c r="L25" s="63" t="n"/>
-      <c r="M25" s="63" t="n"/>
-      <c r="N25" s="81" t="n"/>
+      <c r="L25" s="107" t="n"/>
+      <c r="M25" s="108" t="n"/>
+      <c r="N25" s="114" t="n"/>
+      <c r="O25" s="101" t="n"/>
+      <c r="P25" s="101" t="n"/>
+      <c r="Q25" s="101" t="n"/>
+      <c r="R25" s="101" t="n"/>
+      <c r="S25" s="101" t="n"/>
     </row>
     <row r="26" ht="15" customHeight="1">
-      <c r="A26" s="102" t="inlineStr">
+      <c r="A26" s="109" t="inlineStr">
         <is>
           <t>B3:3/12</t>
         </is>
       </c>
-      <c r="B26" s="102" t="inlineStr"/>
-      <c r="C26" s="103" t="inlineStr">
+      <c r="B26" s="109" t="inlineStr"/>
+      <c r="C26" s="109" t="inlineStr">
         <is>
           <t>FE 5 Failure Alarm</t>
         </is>
       </c>
-      <c r="D26" s="104" t="inlineStr"/>
-      <c r="E26" s="105" t="inlineStr"/>
-      <c r="F26" s="106" t="inlineStr"/>
-      <c r="G26" s="107" t="inlineStr"/>
-      <c r="H26" s="108" t="inlineStr"/>
-      <c r="I26" s="109" t="inlineStr"/>
-      <c r="J26" s="108" t="inlineStr"/>
+      <c r="D26" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" s="112" t="inlineStr"/>
+      <c r="H26" s="112" t="inlineStr"/>
+      <c r="I26" s="113" t="inlineStr"/>
+      <c r="J26" s="112" t="inlineStr"/>
       <c r="K26" s="110" t="inlineStr"/>
-      <c r="L26" s="63" t="n"/>
-      <c r="M26" s="63" t="n"/>
-      <c r="N26" s="81" t="n"/>
+      <c r="L26" s="107" t="n"/>
+      <c r="M26" s="108" t="n"/>
+      <c r="N26" s="114" t="n"/>
+      <c r="O26" s="101" t="n"/>
+      <c r="P26" s="101" t="n"/>
+      <c r="Q26" s="101" t="n"/>
+      <c r="R26" s="101" t="n"/>
+      <c r="S26" s="101" t="n"/>
     </row>
     <row r="27" ht="15" customHeight="1">
-      <c r="A27" s="102" t="inlineStr">
+      <c r="A27" s="109" t="inlineStr">
         <is>
           <t>B3:3/13</t>
         </is>
       </c>
-      <c r="B27" s="102" t="inlineStr"/>
-      <c r="C27" s="103" t="inlineStr">
+      <c r="B27" s="109" t="inlineStr"/>
+      <c r="C27" s="109" t="inlineStr">
         <is>
           <t>FE 6 Failure Alarm</t>
         </is>
       </c>
-      <c r="D27" s="104" t="inlineStr"/>
-      <c r="E27" s="105" t="inlineStr"/>
-      <c r="F27" s="106" t="inlineStr"/>
-      <c r="G27" s="107" t="inlineStr"/>
-      <c r="H27" s="108" t="inlineStr"/>
-      <c r="I27" s="109" t="inlineStr"/>
-      <c r="J27" s="108" t="inlineStr"/>
+      <c r="D27" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" s="112" t="inlineStr"/>
+      <c r="H27" s="112" t="inlineStr"/>
+      <c r="I27" s="113" t="inlineStr"/>
+      <c r="J27" s="112" t="inlineStr"/>
       <c r="K27" s="110" t="inlineStr"/>
-      <c r="L27" s="63" t="n"/>
-      <c r="M27" s="63" t="n"/>
-      <c r="N27" s="81" t="n"/>
+      <c r="L27" s="107" t="n"/>
+      <c r="M27" s="108" t="n"/>
+      <c r="N27" s="114" t="n"/>
+      <c r="O27" s="101" t="n"/>
+      <c r="P27" s="101" t="n"/>
+      <c r="Q27" s="101" t="n"/>
+      <c r="R27" s="101" t="n"/>
+      <c r="S27" s="101" t="n"/>
     </row>
     <row r="28" ht="15" customHeight="1">
-      <c r="A28" s="102" t="inlineStr">
+      <c r="A28" s="109" t="inlineStr">
         <is>
           <t>B3:3/14</t>
         </is>
       </c>
-      <c r="B28" s="102" t="inlineStr"/>
-      <c r="C28" s="103" t="inlineStr">
+      <c r="B28" s="109" t="inlineStr"/>
+      <c r="C28" s="109" t="inlineStr">
         <is>
           <t>FE 7 Failure Alarm</t>
         </is>
       </c>
-      <c r="D28" s="104" t="inlineStr"/>
-      <c r="E28" s="105" t="inlineStr"/>
-      <c r="F28" s="106" t="inlineStr"/>
-      <c r="G28" s="107" t="inlineStr"/>
-      <c r="H28" s="108" t="inlineStr"/>
-      <c r="I28" s="109" t="inlineStr"/>
-      <c r="J28" s="108" t="inlineStr"/>
+      <c r="D28" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" s="112" t="inlineStr"/>
+      <c r="H28" s="112" t="inlineStr"/>
+      <c r="I28" s="113" t="inlineStr"/>
+      <c r="J28" s="112" t="inlineStr"/>
       <c r="K28" s="110" t="inlineStr"/>
-      <c r="L28" s="63" t="n"/>
-      <c r="M28" s="63" t="n"/>
-      <c r="N28" s="81" t="n"/>
+      <c r="L28" s="107" t="n"/>
+      <c r="M28" s="108" t="n"/>
+      <c r="N28" s="114" t="n"/>
+      <c r="O28" s="101" t="n"/>
+      <c r="P28" s="101" t="n"/>
+      <c r="Q28" s="101" t="n"/>
+      <c r="R28" s="101" t="n"/>
+      <c r="S28" s="101" t="n"/>
     </row>
     <row r="29" ht="15" customHeight="1">
-      <c r="A29" s="102" t="inlineStr">
+      <c r="A29" s="109" t="inlineStr">
         <is>
           <t>B3:3/15</t>
         </is>
       </c>
-      <c r="B29" s="102" t="inlineStr"/>
-      <c r="C29" s="103" t="inlineStr">
+      <c r="B29" s="109" t="inlineStr"/>
+      <c r="C29" s="109" t="inlineStr">
         <is>
           <t>FE 8 Failure Alarm</t>
         </is>
       </c>
-      <c r="D29" s="104" t="inlineStr"/>
-      <c r="E29" s="105" t="inlineStr"/>
-      <c r="F29" s="106" t="inlineStr"/>
-      <c r="G29" s="107" t="inlineStr"/>
-      <c r="H29" s="108" t="inlineStr"/>
-      <c r="I29" s="109" t="inlineStr"/>
-      <c r="J29" s="108" t="inlineStr"/>
+      <c r="D29" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" s="112" t="inlineStr"/>
+      <c r="H29" s="112" t="inlineStr"/>
+      <c r="I29" s="113" t="inlineStr"/>
+      <c r="J29" s="112" t="inlineStr"/>
       <c r="K29" s="110" t="inlineStr"/>
-      <c r="L29" s="63" t="n"/>
-      <c r="M29" s="63" t="n"/>
-      <c r="N29" s="81" t="n"/>
+      <c r="L29" s="107" t="n"/>
+      <c r="M29" s="108" t="n"/>
+      <c r="N29" s="114" t="n"/>
+      <c r="O29" s="101" t="n"/>
+      <c r="P29" s="101" t="n"/>
+      <c r="Q29" s="101" t="n"/>
+      <c r="R29" s="101" t="n"/>
+      <c r="S29" s="101" t="n"/>
     </row>
     <row r="30" ht="15" customHeight="1">
-      <c r="A30" s="102" t="inlineStr">
+      <c r="A30" s="109" t="inlineStr">
         <is>
           <t>B3:4/6</t>
         </is>
       </c>
-      <c r="B30" s="102" t="inlineStr"/>
-      <c r="C30" s="103" t="inlineStr">
+      <c r="B30" s="109" t="inlineStr"/>
+      <c r="C30" s="109" t="inlineStr">
         <is>
           <t>2 Detectors In Alarm Zone 1</t>
         </is>
       </c>
-      <c r="D30" s="104" t="inlineStr"/>
-      <c r="E30" s="105" t="inlineStr"/>
-      <c r="F30" s="106" t="inlineStr"/>
-      <c r="G30" s="107" t="inlineStr"/>
-      <c r="H30" s="108" t="inlineStr"/>
-      <c r="I30" s="109" t="inlineStr"/>
-      <c r="J30" s="108" t="inlineStr"/>
+      <c r="D30" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" s="112" t="inlineStr"/>
+      <c r="H30" s="112" t="inlineStr"/>
+      <c r="I30" s="113" t="inlineStr"/>
+      <c r="J30" s="112" t="inlineStr"/>
       <c r="K30" s="110" t="inlineStr"/>
-      <c r="L30" s="63" t="n"/>
-      <c r="M30" s="63" t="n"/>
-      <c r="N30" s="81" t="n"/>
+      <c r="L30" s="107" t="n"/>
+      <c r="M30" s="108" t="n"/>
+      <c r="N30" s="114" t="n"/>
+      <c r="O30" s="101" t="n"/>
+      <c r="P30" s="101" t="n"/>
+      <c r="Q30" s="101" t="n"/>
+      <c r="R30" s="101" t="n"/>
+      <c r="S30" s="101" t="n"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="102" t="inlineStr">
+      <c r="A31" s="109" t="inlineStr">
         <is>
           <t>B3:4/5</t>
         </is>
       </c>
-      <c r="B31" s="102" t="inlineStr"/>
-      <c r="C31" s="103" t="inlineStr">
+      <c r="B31" s="109" t="inlineStr"/>
+      <c r="C31" s="109" t="inlineStr">
         <is>
           <t>2 Detectors In Alarm Zone 2</t>
         </is>
       </c>
-      <c r="D31" s="104" t="inlineStr"/>
-      <c r="E31" s="105" t="inlineStr"/>
-      <c r="F31" s="106" t="inlineStr"/>
-      <c r="G31" s="107" t="inlineStr"/>
-      <c r="H31" s="108" t="inlineStr"/>
-      <c r="I31" s="109" t="inlineStr"/>
-      <c r="J31" s="108" t="inlineStr"/>
+      <c r="D31" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" s="112" t="inlineStr"/>
+      <c r="H31" s="112" t="inlineStr"/>
+      <c r="I31" s="113" t="inlineStr"/>
+      <c r="J31" s="112" t="inlineStr"/>
       <c r="K31" s="110" t="inlineStr"/>
-      <c r="L31" s="63" t="n"/>
-      <c r="M31" s="63" t="n"/>
-      <c r="N31" s="81" t="n"/>
+      <c r="L31" s="107" t="n"/>
+      <c r="M31" s="108" t="n"/>
+      <c r="N31" s="114" t="n"/>
+      <c r="O31" s="101" t="n"/>
+      <c r="P31" s="101" t="n"/>
+      <c r="Q31" s="101" t="n"/>
+      <c r="R31" s="101" t="n"/>
+      <c r="S31" s="101" t="n"/>
     </row>
     <row r="32" ht="15" customHeight="1">
-      <c r="A32" s="102" t="inlineStr">
+      <c r="A32" s="109" t="inlineStr">
         <is>
           <t>B3:10/0</t>
         </is>
       </c>
-      <c r="B32" s="102" t="inlineStr"/>
-      <c r="C32" s="103" t="inlineStr">
+      <c r="B32" s="109" t="inlineStr"/>
+      <c r="C32" s="109" t="inlineStr">
         <is>
           <t>ESD Alarm to Office PLC</t>
         </is>
       </c>
-      <c r="D32" s="104" t="inlineStr"/>
-      <c r="E32" s="105" t="inlineStr"/>
-      <c r="F32" s="106" t="inlineStr"/>
-      <c r="G32" s="107" t="inlineStr"/>
-      <c r="H32" s="108" t="inlineStr"/>
-      <c r="I32" s="109" t="inlineStr"/>
-      <c r="J32" s="108" t="inlineStr"/>
+      <c r="D32" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" s="111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" s="112" t="inlineStr"/>
+      <c r="H32" s="112" t="inlineStr"/>
+      <c r="I32" s="113" t="inlineStr"/>
+      <c r="J32" s="112" t="inlineStr"/>
       <c r="K32" s="110" t="inlineStr"/>
-      <c r="L32" s="63" t="n"/>
-      <c r="M32" s="63" t="n"/>
-      <c r="N32" s="81" t="n"/>
+      <c r="L32" s="107" t="n"/>
+      <c r="M32" s="108" t="n"/>
+      <c r="N32" s="114" t="n"/>
+      <c r="O32" s="101" t="n"/>
+      <c r="P32" s="101" t="n"/>
+      <c r="Q32" s="101" t="n"/>
+      <c r="R32" s="101" t="n"/>
+      <c r="S32" s="101" t="n"/>
     </row>
     <row r="33" ht="15" customHeight="1">
-      <c r="A33" s="13" t="n"/>
-      <c r="B33" s="14" t="n"/>
-      <c r="C33" s="36" t="n"/>
-      <c r="D33" s="30" t="n"/>
-      <c r="E33" s="14" t="n"/>
-      <c r="F33" s="15" t="n"/>
-      <c r="G33" s="25" t="n"/>
-      <c r="H33" s="26" t="n"/>
-      <c r="I33" s="61" t="n"/>
-      <c r="J33" s="62" t="n"/>
-      <c r="K33" s="63" t="n"/>
-      <c r="L33" s="63" t="n"/>
-      <c r="M33" s="63" t="n"/>
-      <c r="N33" s="81" t="n"/>
+      <c r="A33" s="115" t="n"/>
+      <c r="B33" s="115" t="n"/>
+      <c r="C33" s="116" t="n"/>
+      <c r="D33" s="115" t="n"/>
+      <c r="E33" s="115" t="n"/>
+      <c r="F33" s="117" t="n"/>
+      <c r="G33" s="118" t="n"/>
+      <c r="H33" s="118" t="n"/>
+      <c r="I33" s="119" t="n"/>
+      <c r="J33" s="118" t="n"/>
+      <c r="K33" s="120" t="n"/>
+      <c r="L33" s="107" t="n"/>
+      <c r="M33" s="108" t="n"/>
+      <c r="N33" s="114" t="n"/>
+      <c r="O33" s="101" t="n"/>
+      <c r="P33" s="101" t="n"/>
+      <c r="Q33" s="101" t="n"/>
+      <c r="R33" s="101" t="n"/>
+      <c r="S33" s="101" t="n"/>
     </row>
     <row r="34" ht="15" customHeight="1">
-      <c r="A34" s="13" t="n"/>
-      <c r="B34" s="14" t="n"/>
-      <c r="C34" s="36" t="n"/>
-      <c r="D34" s="30" t="n"/>
-      <c r="E34" s="14" t="n"/>
-      <c r="F34" s="15" t="n"/>
-      <c r="G34" s="25" t="n"/>
-      <c r="H34" s="26" t="n"/>
-      <c r="I34" s="61" t="n"/>
-      <c r="J34" s="62" t="n"/>
-      <c r="K34" s="63" t="n"/>
-      <c r="L34" s="63" t="n"/>
-      <c r="M34" s="63" t="n"/>
-      <c r="N34" s="81" t="n"/>
+      <c r="A34" s="115" t="n"/>
+      <c r="B34" s="115" t="n"/>
+      <c r="C34" s="116" t="n"/>
+      <c r="D34" s="115" t="n"/>
+      <c r="E34" s="115" t="n"/>
+      <c r="F34" s="117" t="n"/>
+      <c r="G34" s="118" t="n"/>
+      <c r="H34" s="118" t="n"/>
+      <c r="I34" s="119" t="n"/>
+      <c r="J34" s="118" t="n"/>
+      <c r="K34" s="120" t="n"/>
+      <c r="L34" s="107" t="n"/>
+      <c r="M34" s="108" t="n"/>
+      <c r="N34" s="114" t="n"/>
+      <c r="O34" s="101" t="n"/>
+      <c r="P34" s="101" t="n"/>
+      <c r="Q34" s="101" t="n"/>
+      <c r="R34" s="101" t="n"/>
+      <c r="S34" s="101" t="n"/>
     </row>
     <row r="35" ht="15" customHeight="1">
-      <c r="A35" s="13" t="n"/>
-      <c r="B35" s="14" t="n"/>
-      <c r="C35" s="36" t="n"/>
-      <c r="D35" s="30" t="n"/>
-      <c r="E35" s="14" t="n"/>
-      <c r="F35" s="15" t="n"/>
-      <c r="G35" s="25" t="n"/>
-      <c r="H35" s="26" t="n"/>
-      <c r="I35" s="61" t="n"/>
-      <c r="J35" s="62" t="n"/>
-      <c r="K35" s="63" t="n"/>
-      <c r="L35" s="63" t="n"/>
-      <c r="M35" s="63" t="n"/>
-      <c r="N35" s="81" t="n"/>
+      <c r="A35" s="115" t="n"/>
+      <c r="B35" s="115" t="n"/>
+      <c r="C35" s="116" t="n"/>
+      <c r="D35" s="115" t="n"/>
+      <c r="E35" s="115" t="n"/>
+      <c r="F35" s="117" t="n"/>
+      <c r="G35" s="118" t="n"/>
+      <c r="H35" s="118" t="n"/>
+      <c r="I35" s="119" t="n"/>
+      <c r="J35" s="118" t="n"/>
+      <c r="K35" s="120" t="n"/>
+      <c r="L35" s="107" t="n"/>
+      <c r="M35" s="108" t="n"/>
+      <c r="N35" s="114" t="n"/>
+      <c r="O35" s="101" t="n"/>
+      <c r="P35" s="101" t="n"/>
+      <c r="Q35" s="101" t="n"/>
+      <c r="R35" s="101" t="n"/>
+      <c r="S35" s="101" t="n"/>
     </row>
     <row r="36" ht="15" customHeight="1">
-      <c r="A36" s="13" t="n"/>
-      <c r="B36" s="14" t="n"/>
-      <c r="C36" s="36" t="n"/>
-      <c r="D36" s="30" t="n"/>
-      <c r="E36" s="14" t="n"/>
-      <c r="F36" s="15" t="n"/>
-      <c r="G36" s="25" t="n"/>
-      <c r="H36" s="26" t="n"/>
-      <c r="I36" s="61" t="n"/>
-      <c r="J36" s="62" t="n"/>
-      <c r="K36" s="63" t="n"/>
-      <c r="L36" s="63" t="n"/>
-      <c r="M36" s="63" t="n"/>
-      <c r="N36" s="81" t="n"/>
+      <c r="A36" s="115" t="n"/>
+      <c r="B36" s="115" t="n"/>
+      <c r="C36" s="116" t="n"/>
+      <c r="D36" s="115" t="n"/>
+      <c r="E36" s="115" t="n"/>
+      <c r="F36" s="117" t="n"/>
+      <c r="G36" s="118" t="n"/>
+      <c r="H36" s="118" t="n"/>
+      <c r="I36" s="119" t="n"/>
+      <c r="J36" s="118" t="n"/>
+      <c r="K36" s="120" t="n"/>
+      <c r="L36" s="107" t="n"/>
+      <c r="M36" s="108" t="n"/>
+      <c r="N36" s="114" t="n"/>
+      <c r="O36" s="101" t="n"/>
+      <c r="P36" s="101" t="n"/>
+      <c r="Q36" s="101" t="n"/>
+      <c r="R36" s="101" t="n"/>
+      <c r="S36" s="101" t="n"/>
     </row>
     <row r="37" ht="15" customHeight="1">
-      <c r="A37" s="13" t="n"/>
-      <c r="B37" s="14" t="n"/>
-      <c r="C37" s="36" t="n"/>
-      <c r="D37" s="30" t="n"/>
-      <c r="E37" s="14" t="n"/>
-      <c r="F37" s="15" t="n"/>
-      <c r="G37" s="25" t="n"/>
-      <c r="H37" s="26" t="n"/>
-      <c r="I37" s="61" t="n"/>
-      <c r="J37" s="62" t="n"/>
-      <c r="K37" s="63" t="n"/>
-      <c r="L37" s="63" t="n"/>
-      <c r="M37" s="63" t="n"/>
-      <c r="N37" s="81" t="n"/>
+      <c r="A37" s="115" t="n"/>
+      <c r="B37" s="115" t="n"/>
+      <c r="C37" s="116" t="n"/>
+      <c r="D37" s="115" t="n"/>
+      <c r="E37" s="115" t="n"/>
+      <c r="F37" s="117" t="n"/>
+      <c r="G37" s="118" t="n"/>
+      <c r="H37" s="118" t="n"/>
+      <c r="I37" s="119" t="n"/>
+      <c r="J37" s="118" t="n"/>
+      <c r="K37" s="120" t="n"/>
+      <c r="L37" s="107" t="n"/>
+      <c r="M37" s="108" t="n"/>
+      <c r="N37" s="114" t="n"/>
+      <c r="O37" s="101" t="n"/>
+      <c r="P37" s="101" t="n"/>
+      <c r="Q37" s="101" t="n"/>
+      <c r="R37" s="101" t="n"/>
+      <c r="S37" s="101" t="n"/>
     </row>
     <row r="38" ht="15" customHeight="1">
-      <c r="A38" s="13" t="n"/>
-      <c r="B38" s="14" t="n"/>
-      <c r="C38" s="36" t="n"/>
-      <c r="D38" s="30" t="n"/>
-      <c r="E38" s="14" t="n"/>
-      <c r="F38" s="15" t="n"/>
-      <c r="G38" s="25" t="n"/>
-      <c r="H38" s="26" t="n"/>
-      <c r="I38" s="61" t="n"/>
-      <c r="J38" s="62" t="n"/>
-      <c r="K38" s="63" t="n"/>
-      <c r="L38" s="63" t="n"/>
-      <c r="M38" s="63" t="n"/>
-      <c r="N38" s="81" t="n"/>
+      <c r="A38" s="115" t="n"/>
+      <c r="B38" s="115" t="n"/>
+      <c r="C38" s="116" t="n"/>
+      <c r="D38" s="115" t="n"/>
+      <c r="E38" s="115" t="n"/>
+      <c r="F38" s="117" t="n"/>
+      <c r="G38" s="118" t="n"/>
+      <c r="H38" s="118" t="n"/>
+      <c r="I38" s="119" t="n"/>
+      <c r="J38" s="118" t="n"/>
+      <c r="K38" s="120" t="n"/>
+      <c r="L38" s="107" t="n"/>
+      <c r="M38" s="108" t="n"/>
+      <c r="N38" s="114" t="n"/>
+      <c r="O38" s="101" t="n"/>
+      <c r="P38" s="101" t="n"/>
+      <c r="Q38" s="101" t="n"/>
+      <c r="R38" s="101" t="n"/>
+      <c r="S38" s="101" t="n"/>
     </row>
     <row r="39" ht="15" customHeight="1">
-      <c r="A39" s="13" t="n"/>
-      <c r="B39" s="14" t="n"/>
-      <c r="C39" s="36" t="n"/>
-      <c r="D39" s="30" t="n"/>
-      <c r="E39" s="14" t="n"/>
-      <c r="F39" s="15" t="n"/>
-      <c r="G39" s="25" t="n"/>
-      <c r="H39" s="26" t="n"/>
-      <c r="I39" s="61" t="n"/>
-      <c r="J39" s="62" t="n"/>
-      <c r="K39" s="63" t="n"/>
-      <c r="L39" s="63" t="n"/>
-      <c r="M39" s="63" t="n"/>
-      <c r="N39" s="81" t="n"/>
+      <c r="A39" s="115" t="n"/>
+      <c r="B39" s="115" t="n"/>
+      <c r="C39" s="116" t="n"/>
+      <c r="D39" s="115" t="n"/>
+      <c r="E39" s="115" t="n"/>
+      <c r="F39" s="117" t="n"/>
+      <c r="G39" s="118" t="n"/>
+      <c r="H39" s="118" t="n"/>
+      <c r="I39" s="119" t="n"/>
+      <c r="J39" s="118" t="n"/>
+      <c r="K39" s="120" t="n"/>
+      <c r="L39" s="107" t="n"/>
+      <c r="M39" s="108" t="n"/>
+      <c r="N39" s="114" t="n"/>
+      <c r="O39" s="101" t="n"/>
+      <c r="P39" s="101" t="n"/>
+      <c r="Q39" s="101" t="n"/>
+      <c r="R39" s="101" t="n"/>
+      <c r="S39" s="101" t="n"/>
     </row>
     <row r="40" ht="15" customHeight="1">
-      <c r="A40" s="13" t="n"/>
-      <c r="B40" s="14" t="n"/>
-      <c r="C40" s="36" t="n"/>
-      <c r="D40" s="30" t="n"/>
-      <c r="E40" s="14" t="n"/>
-      <c r="F40" s="15" t="n"/>
-      <c r="G40" s="25" t="n"/>
-      <c r="H40" s="26" t="n"/>
-      <c r="I40" s="61" t="n"/>
-      <c r="J40" s="62" t="n"/>
-      <c r="K40" s="63" t="n"/>
-      <c r="L40" s="63" t="n"/>
-      <c r="M40" s="63" t="n"/>
-      <c r="N40" s="81" t="n"/>
+      <c r="A40" s="115" t="n"/>
+      <c r="B40" s="115" t="n"/>
+      <c r="C40" s="116" t="n"/>
+      <c r="D40" s="115" t="n"/>
+      <c r="E40" s="115" t="n"/>
+      <c r="F40" s="117" t="n"/>
+      <c r="G40" s="118" t="n"/>
+      <c r="H40" s="118" t="n"/>
+      <c r="I40" s="119" t="n"/>
+      <c r="J40" s="118" t="n"/>
+      <c r="K40" s="120" t="n"/>
+      <c r="L40" s="107" t="n"/>
+      <c r="M40" s="108" t="n"/>
+      <c r="N40" s="114" t="n"/>
+      <c r="O40" s="101" t="n"/>
+      <c r="P40" s="101" t="n"/>
+      <c r="Q40" s="101" t="n"/>
+      <c r="R40" s="101" t="n"/>
+      <c r="S40" s="101" t="n"/>
     </row>
     <row r="41" ht="15" customHeight="1">
-      <c r="A41" s="13" t="n"/>
-      <c r="B41" s="14" t="n"/>
-      <c r="C41" s="36" t="n"/>
-      <c r="D41" s="30" t="n"/>
-      <c r="E41" s="14" t="n"/>
-      <c r="F41" s="15" t="n"/>
-      <c r="G41" s="25" t="n"/>
-      <c r="H41" s="26" t="n"/>
-      <c r="I41" s="61" t="n"/>
-      <c r="J41" s="62" t="n"/>
-      <c r="K41" s="63" t="n"/>
-      <c r="L41" s="63" t="n"/>
-      <c r="M41" s="63" t="n"/>
-      <c r="N41" s="81" t="n"/>
+      <c r="A41" s="115" t="n"/>
+      <c r="B41" s="115" t="n"/>
+      <c r="C41" s="116" t="n"/>
+      <c r="D41" s="115" t="n"/>
+      <c r="E41" s="115" t="n"/>
+      <c r="F41" s="117" t="n"/>
+      <c r="G41" s="118" t="n"/>
+      <c r="H41" s="118" t="n"/>
+      <c r="I41" s="119" t="n"/>
+      <c r="J41" s="118" t="n"/>
+      <c r="K41" s="120" t="n"/>
+      <c r="L41" s="107" t="n"/>
+      <c r="M41" s="108" t="n"/>
+      <c r="N41" s="114" t="n"/>
+      <c r="O41" s="101" t="n"/>
+      <c r="P41" s="101" t="n"/>
+      <c r="Q41" s="101" t="n"/>
+      <c r="R41" s="101" t="n"/>
+      <c r="S41" s="101" t="n"/>
     </row>
     <row r="42" ht="15" customHeight="1">
-      <c r="A42" s="13" t="n"/>
-      <c r="B42" s="14" t="n"/>
-      <c r="C42" s="36" t="n"/>
-      <c r="D42" s="30" t="n"/>
-      <c r="E42" s="14" t="n"/>
-      <c r="F42" s="15" t="n"/>
-      <c r="G42" s="25" t="n"/>
-      <c r="H42" s="26" t="n"/>
-      <c r="I42" s="61" t="n"/>
-      <c r="J42" s="62" t="n"/>
-      <c r="K42" s="63" t="n"/>
-      <c r="L42" s="63" t="n"/>
-      <c r="M42" s="63" t="n"/>
-      <c r="N42" s="81" t="n"/>
+      <c r="A42" s="115" t="n"/>
+      <c r="B42" s="115" t="n"/>
+      <c r="C42" s="116" t="n"/>
+      <c r="D42" s="115" t="n"/>
+      <c r="E42" s="115" t="n"/>
+      <c r="F42" s="117" t="n"/>
+      <c r="G42" s="118" t="n"/>
+      <c r="H42" s="118" t="n"/>
+      <c r="I42" s="119" t="n"/>
+      <c r="J42" s="118" t="n"/>
+      <c r="K42" s="120" t="n"/>
+      <c r="L42" s="107" t="n"/>
+      <c r="M42" s="108" t="n"/>
+      <c r="N42" s="114" t="n"/>
+      <c r="O42" s="101" t="n"/>
+      <c r="P42" s="101" t="n"/>
+      <c r="Q42" s="101" t="n"/>
+      <c r="R42" s="101" t="n"/>
+      <c r="S42" s="101" t="n"/>
     </row>
     <row r="43" ht="15" customHeight="1">
-      <c r="A43" s="13" t="n"/>
-      <c r="B43" s="14" t="n"/>
-      <c r="C43" s="36" t="n"/>
-      <c r="D43" s="30" t="n"/>
-      <c r="E43" s="14" t="n"/>
-      <c r="F43" s="15" t="n"/>
-      <c r="G43" s="25" t="n"/>
-      <c r="H43" s="26" t="n"/>
-      <c r="I43" s="61" t="n"/>
-      <c r="J43" s="62" t="n"/>
-      <c r="K43" s="63" t="n"/>
-      <c r="L43" s="63" t="n"/>
-      <c r="M43" s="63" t="n"/>
-      <c r="N43" s="81" t="n"/>
+      <c r="A43" s="115" t="n"/>
+      <c r="B43" s="115" t="n"/>
+      <c r="C43" s="116" t="n"/>
+      <c r="D43" s="115" t="n"/>
+      <c r="E43" s="115" t="n"/>
+      <c r="F43" s="117" t="n"/>
+      <c r="G43" s="118" t="n"/>
+      <c r="H43" s="118" t="n"/>
+      <c r="I43" s="119" t="n"/>
+      <c r="J43" s="118" t="n"/>
+      <c r="K43" s="120" t="n"/>
+      <c r="L43" s="107" t="n"/>
+      <c r="M43" s="108" t="n"/>
+      <c r="N43" s="114" t="n"/>
+      <c r="O43" s="101" t="n"/>
+      <c r="P43" s="101" t="n"/>
+      <c r="Q43" s="101" t="n"/>
+      <c r="R43" s="101" t="n"/>
+      <c r="S43" s="101" t="n"/>
     </row>
     <row r="44" ht="15" customHeight="1">
-      <c r="A44" s="13" t="n"/>
-      <c r="B44" s="14" t="n"/>
-      <c r="C44" s="36" t="n"/>
-      <c r="D44" s="30" t="n"/>
-      <c r="E44" s="14" t="n"/>
-      <c r="F44" s="15" t="n"/>
-      <c r="G44" s="25" t="n"/>
-      <c r="H44" s="26" t="n"/>
-      <c r="I44" s="61" t="n"/>
-      <c r="J44" s="62" t="n"/>
-      <c r="K44" s="63" t="n"/>
-      <c r="L44" s="63" t="n"/>
-      <c r="M44" s="63" t="n"/>
-      <c r="N44" s="81" t="n"/>
+      <c r="A44" s="115" t="n"/>
+      <c r="B44" s="115" t="n"/>
+      <c r="C44" s="116" t="n"/>
+      <c r="D44" s="115" t="n"/>
+      <c r="E44" s="115" t="n"/>
+      <c r="F44" s="117" t="n"/>
+      <c r="G44" s="118" t="n"/>
+      <c r="H44" s="118" t="n"/>
+      <c r="I44" s="119" t="n"/>
+      <c r="J44" s="118" t="n"/>
+      <c r="K44" s="120" t="n"/>
+      <c r="L44" s="107" t="n"/>
+      <c r="M44" s="108" t="n"/>
+      <c r="N44" s="114" t="n"/>
+      <c r="O44" s="101" t="n"/>
+      <c r="P44" s="101" t="n"/>
+      <c r="Q44" s="101" t="n"/>
+      <c r="R44" s="101" t="n"/>
+      <c r="S44" s="101" t="n"/>
     </row>
     <row r="45" ht="15" customHeight="1">
-      <c r="A45" s="13" t="n"/>
-      <c r="B45" s="14" t="n"/>
-      <c r="C45" s="36" t="n"/>
-      <c r="D45" s="30" t="n"/>
-      <c r="E45" s="14" t="n"/>
-      <c r="F45" s="15" t="n"/>
-      <c r="G45" s="25" t="n"/>
-      <c r="H45" s="26" t="n"/>
-      <c r="I45" s="61" t="n"/>
-      <c r="J45" s="62" t="n"/>
-      <c r="K45" s="63" t="n"/>
-      <c r="L45" s="63" t="n"/>
-      <c r="M45" s="63" t="n"/>
-      <c r="N45" s="81" t="n"/>
+      <c r="A45" s="115" t="n"/>
+      <c r="B45" s="115" t="n"/>
+      <c r="C45" s="116" t="n"/>
+      <c r="D45" s="115" t="n"/>
+      <c r="E45" s="115" t="n"/>
+      <c r="F45" s="117" t="n"/>
+      <c r="G45" s="118" t="n"/>
+      <c r="H45" s="118" t="n"/>
+      <c r="I45" s="119" t="n"/>
+      <c r="J45" s="118" t="n"/>
+      <c r="K45" s="120" t="n"/>
+      <c r="L45" s="107" t="n"/>
+      <c r="M45" s="108" t="n"/>
+      <c r="N45" s="114" t="n"/>
+      <c r="O45" s="101" t="n"/>
+      <c r="P45" s="101" t="n"/>
+      <c r="Q45" s="101" t="n"/>
+      <c r="R45" s="101" t="n"/>
+      <c r="S45" s="101" t="n"/>
     </row>
     <row r="46" ht="15" customHeight="1">
-      <c r="A46" s="13" t="n"/>
-      <c r="B46" s="14" t="n"/>
-      <c r="C46" s="36" t="n"/>
-      <c r="D46" s="30" t="n"/>
-      <c r="E46" s="14" t="n"/>
-      <c r="F46" s="15" t="n"/>
-      <c r="G46" s="25" t="n"/>
-      <c r="H46" s="26" t="n"/>
-      <c r="I46" s="61" t="n"/>
-      <c r="J46" s="62" t="n"/>
-      <c r="K46" s="63" t="n"/>
-      <c r="L46" s="63" t="n"/>
-      <c r="M46" s="63" t="n"/>
-      <c r="N46" s="81" t="n"/>
+      <c r="A46" s="115" t="n"/>
+      <c r="B46" s="115" t="n"/>
+      <c r="C46" s="116" t="n"/>
+      <c r="D46" s="115" t="n"/>
+      <c r="E46" s="115" t="n"/>
+      <c r="F46" s="117" t="n"/>
+      <c r="G46" s="118" t="n"/>
+      <c r="H46" s="118" t="n"/>
+      <c r="I46" s="119" t="n"/>
+      <c r="J46" s="118" t="n"/>
+      <c r="K46" s="120" t="n"/>
+      <c r="L46" s="107" t="n"/>
+      <c r="M46" s="108" t="n"/>
+      <c r="N46" s="114" t="n"/>
+      <c r="O46" s="101" t="n"/>
+      <c r="P46" s="101" t="n"/>
+      <c r="Q46" s="101" t="n"/>
+      <c r="R46" s="101" t="n"/>
+      <c r="S46" s="101" t="n"/>
     </row>
     <row r="47" ht="15" customHeight="1">
-      <c r="A47" s="13" t="n"/>
-      <c r="B47" s="14" t="n"/>
-      <c r="C47" s="36" t="n"/>
-      <c r="D47" s="30" t="n"/>
-      <c r="E47" s="14" t="n"/>
-      <c r="F47" s="15" t="n"/>
-      <c r="G47" s="25" t="n"/>
-      <c r="H47" s="26" t="n"/>
-      <c r="I47" s="61" t="n"/>
-      <c r="J47" s="62" t="n"/>
-      <c r="K47" s="63" t="n"/>
-      <c r="L47" s="63" t="n"/>
-      <c r="M47" s="63" t="n"/>
-      <c r="N47" s="81" t="n"/>
+      <c r="A47" s="115" t="n"/>
+      <c r="B47" s="115" t="n"/>
+      <c r="C47" s="116" t="n"/>
+      <c r="D47" s="115" t="n"/>
+      <c r="E47" s="115" t="n"/>
+      <c r="F47" s="117" t="n"/>
+      <c r="G47" s="118" t="n"/>
+      <c r="H47" s="118" t="n"/>
+      <c r="I47" s="119" t="n"/>
+      <c r="J47" s="118" t="n"/>
+      <c r="K47" s="120" t="n"/>
+      <c r="L47" s="107" t="n"/>
+      <c r="M47" s="108" t="n"/>
+      <c r="N47" s="114" t="n"/>
+      <c r="O47" s="101" t="n"/>
+      <c r="P47" s="101" t="n"/>
+      <c r="Q47" s="101" t="n"/>
+      <c r="R47" s="101" t="n"/>
+      <c r="S47" s="101" t="n"/>
     </row>
     <row r="48" ht="15" customHeight="1">
-      <c r="A48" s="13" t="n"/>
-      <c r="B48" s="14" t="n"/>
-      <c r="C48" s="36" t="n"/>
-      <c r="D48" s="30" t="n"/>
-      <c r="E48" s="14" t="n"/>
-      <c r="F48" s="15" t="n"/>
-      <c r="G48" s="25" t="n"/>
-      <c r="H48" s="26" t="n"/>
-      <c r="I48" s="61" t="n"/>
-      <c r="J48" s="62" t="n"/>
-      <c r="K48" s="63" t="n"/>
-      <c r="L48" s="63" t="n"/>
-      <c r="M48" s="63" t="n"/>
-      <c r="N48" s="81" t="n"/>
+      <c r="A48" s="115" t="n"/>
+      <c r="B48" s="115" t="n"/>
+      <c r="C48" s="116" t="n"/>
+      <c r="D48" s="115" t="n"/>
+      <c r="E48" s="115" t="n"/>
+      <c r="F48" s="117" t="n"/>
+      <c r="G48" s="118" t="n"/>
+      <c r="H48" s="118" t="n"/>
+      <c r="I48" s="119" t="n"/>
+      <c r="J48" s="118" t="n"/>
+      <c r="K48" s="120" t="n"/>
+      <c r="L48" s="107" t="n"/>
+      <c r="M48" s="108" t="n"/>
+      <c r="N48" s="114" t="n"/>
+      <c r="O48" s="101" t="n"/>
+      <c r="P48" s="101" t="n"/>
+      <c r="Q48" s="101" t="n"/>
+      <c r="R48" s="101" t="n"/>
+      <c r="S48" s="101" t="n"/>
     </row>
     <row r="49" ht="15" customHeight="1">
-      <c r="A49" s="13" t="n"/>
-      <c r="B49" s="14" t="n"/>
-      <c r="C49" s="36" t="n"/>
-      <c r="D49" s="30" t="n"/>
-      <c r="E49" s="14" t="n"/>
-      <c r="F49" s="15" t="n"/>
-      <c r="G49" s="25" t="n"/>
-      <c r="H49" s="26" t="n"/>
-      <c r="I49" s="61" t="n"/>
-      <c r="J49" s="62" t="n"/>
-      <c r="K49" s="63" t="n"/>
-      <c r="L49" s="63" t="n"/>
-      <c r="M49" s="63" t="n"/>
-      <c r="N49" s="81" t="n"/>
+      <c r="A49" s="115" t="n"/>
+      <c r="B49" s="115" t="n"/>
+      <c r="C49" s="116" t="n"/>
+      <c r="D49" s="115" t="n"/>
+      <c r="E49" s="115" t="n"/>
+      <c r="F49" s="117" t="n"/>
+      <c r="G49" s="118" t="n"/>
+      <c r="H49" s="118" t="n"/>
+      <c r="I49" s="119" t="n"/>
+      <c r="J49" s="118" t="n"/>
+      <c r="K49" s="120" t="n"/>
+      <c r="L49" s="107" t="n"/>
+      <c r="M49" s="108" t="n"/>
+      <c r="N49" s="114" t="n"/>
+      <c r="O49" s="101" t="n"/>
+      <c r="P49" s="101" t="n"/>
+      <c r="Q49" s="101" t="n"/>
+      <c r="R49" s="101" t="n"/>
+      <c r="S49" s="101" t="n"/>
     </row>
     <row r="50" ht="15" customHeight="1">
-      <c r="A50" s="13" t="n"/>
-      <c r="B50" s="14" t="n"/>
-      <c r="C50" s="36" t="n"/>
-      <c r="D50" s="30" t="n"/>
-      <c r="E50" s="14" t="n"/>
-      <c r="F50" s="15" t="n"/>
-      <c r="G50" s="25" t="n"/>
-      <c r="H50" s="26" t="n"/>
-      <c r="I50" s="61" t="n"/>
-      <c r="J50" s="62" t="n"/>
-      <c r="K50" s="63" t="n"/>
-      <c r="L50" s="63" t="n"/>
-      <c r="M50" s="63" t="n"/>
-      <c r="N50" s="81" t="n"/>
+      <c r="A50" s="115" t="n"/>
+      <c r="B50" s="115" t="n"/>
+      <c r="C50" s="116" t="n"/>
+      <c r="D50" s="115" t="n"/>
+      <c r="E50" s="115" t="n"/>
+      <c r="F50" s="117" t="n"/>
+      <c r="G50" s="118" t="n"/>
+      <c r="H50" s="118" t="n"/>
+      <c r="I50" s="119" t="n"/>
+      <c r="J50" s="118" t="n"/>
+      <c r="K50" s="120" t="n"/>
+      <c r="L50" s="107" t="n"/>
+      <c r="M50" s="108" t="n"/>
+      <c r="N50" s="114" t="n"/>
+      <c r="O50" s="101" t="n"/>
+      <c r="P50" s="101" t="n"/>
+      <c r="Q50" s="101" t="n"/>
+      <c r="R50" s="101" t="n"/>
+      <c r="S50" s="101" t="n"/>
     </row>
     <row r="51" ht="15" customHeight="1">
-      <c r="A51" s="13" t="n"/>
-      <c r="B51" s="14" t="n"/>
-      <c r="C51" s="36" t="n"/>
-      <c r="D51" s="30" t="n"/>
-      <c r="E51" s="14" t="n"/>
-      <c r="F51" s="15" t="n"/>
-      <c r="G51" s="25" t="n"/>
-      <c r="H51" s="26" t="n"/>
-      <c r="I51" s="61" t="n"/>
-      <c r="J51" s="62" t="n"/>
-      <c r="K51" s="63" t="n"/>
-      <c r="L51" s="63" t="n"/>
-      <c r="M51" s="63" t="n"/>
-      <c r="N51" s="81" t="n"/>
+      <c r="A51" s="115" t="n"/>
+      <c r="B51" s="115" t="n"/>
+      <c r="C51" s="116" t="n"/>
+      <c r="D51" s="115" t="n"/>
+      <c r="E51" s="115" t="n"/>
+      <c r="F51" s="117" t="n"/>
+      <c r="G51" s="118" t="n"/>
+      <c r="H51" s="118" t="n"/>
+      <c r="I51" s="119" t="n"/>
+      <c r="J51" s="118" t="n"/>
+      <c r="K51" s="120" t="n"/>
+      <c r="L51" s="107" t="n"/>
+      <c r="M51" s="108" t="n"/>
+      <c r="N51" s="114" t="n"/>
+      <c r="O51" s="101" t="n"/>
+      <c r="P51" s="101" t="n"/>
+      <c r="Q51" s="101" t="n"/>
+      <c r="R51" s="101" t="n"/>
+      <c r="S51" s="101" t="n"/>
     </row>
     <row r="52" ht="15" customHeight="1">
-      <c r="A52" s="13" t="n"/>
-      <c r="B52" s="14" t="n"/>
-      <c r="C52" s="36" t="n"/>
-      <c r="D52" s="30" t="n"/>
-      <c r="E52" s="14" t="n"/>
-      <c r="F52" s="15" t="n"/>
-      <c r="G52" s="25" t="n"/>
-      <c r="H52" s="26" t="n"/>
-      <c r="I52" s="61" t="n"/>
-      <c r="J52" s="62" t="n"/>
-      <c r="K52" s="63" t="n"/>
-      <c r="L52" s="63" t="n"/>
-      <c r="M52" s="63" t="n"/>
-      <c r="N52" s="81" t="n"/>
+      <c r="A52" s="115" t="n"/>
+      <c r="B52" s="115" t="n"/>
+      <c r="C52" s="116" t="n"/>
+      <c r="D52" s="115" t="n"/>
+      <c r="E52" s="115" t="n"/>
+      <c r="F52" s="117" t="n"/>
+      <c r="G52" s="118" t="n"/>
+      <c r="H52" s="118" t="n"/>
+      <c r="I52" s="119" t="n"/>
+      <c r="J52" s="118" t="n"/>
+      <c r="K52" s="120" t="n"/>
+      <c r="L52" s="107" t="n"/>
+      <c r="M52" s="108" t="n"/>
+      <c r="N52" s="114" t="n"/>
+      <c r="O52" s="101" t="n"/>
+      <c r="P52" s="101" t="n"/>
+      <c r="Q52" s="101" t="n"/>
+      <c r="R52" s="101" t="n"/>
+      <c r="S52" s="101" t="n"/>
     </row>
     <row r="53" ht="15" customHeight="1">
-      <c r="A53" s="13" t="n"/>
-      <c r="B53" s="14" t="n"/>
-      <c r="C53" s="36" t="n"/>
-      <c r="D53" s="30" t="n"/>
-      <c r="E53" s="14" t="n"/>
-      <c r="F53" s="15" t="n"/>
-      <c r="G53" s="25" t="n"/>
-      <c r="H53" s="26" t="n"/>
-      <c r="I53" s="61" t="n"/>
-      <c r="J53" s="62" t="n"/>
-      <c r="K53" s="63" t="n"/>
-      <c r="L53" s="63" t="n"/>
-      <c r="M53" s="63" t="n"/>
-      <c r="N53" s="81" t="n"/>
+      <c r="A53" s="115" t="n"/>
+      <c r="B53" s="115" t="n"/>
+      <c r="C53" s="116" t="n"/>
+      <c r="D53" s="115" t="n"/>
+      <c r="E53" s="115" t="n"/>
+      <c r="F53" s="117" t="n"/>
+      <c r="G53" s="118" t="n"/>
+      <c r="H53" s="118" t="n"/>
+      <c r="I53" s="119" t="n"/>
+      <c r="J53" s="118" t="n"/>
+      <c r="K53" s="120" t="n"/>
+      <c r="L53" s="107" t="n"/>
+      <c r="M53" s="108" t="n"/>
+      <c r="N53" s="114" t="n"/>
+      <c r="O53" s="101" t="n"/>
+      <c r="P53" s="101" t="n"/>
+      <c r="Q53" s="101" t="n"/>
+      <c r="R53" s="101" t="n"/>
+      <c r="S53" s="101" t="n"/>
     </row>
     <row r="54" ht="15" customHeight="1">
-      <c r="A54" s="13" t="n"/>
-      <c r="B54" s="14" t="n"/>
-      <c r="C54" s="36" t="n"/>
-      <c r="D54" s="30" t="n"/>
-      <c r="E54" s="14" t="n"/>
-      <c r="F54" s="15" t="n"/>
-      <c r="G54" s="25" t="n"/>
-      <c r="H54" s="26" t="n"/>
-      <c r="I54" s="61" t="n"/>
-      <c r="J54" s="62" t="n"/>
-      <c r="K54" s="63" t="n"/>
-      <c r="L54" s="63" t="n"/>
-      <c r="M54" s="63" t="n"/>
-      <c r="N54" s="81" t="n"/>
+      <c r="A54" s="115" t="n"/>
+      <c r="B54" s="115" t="n"/>
+      <c r="C54" s="116" t="n"/>
+      <c r="D54" s="115" t="n"/>
+      <c r="E54" s="115" t="n"/>
+      <c r="F54" s="117" t="n"/>
+      <c r="G54" s="118" t="n"/>
+      <c r="H54" s="118" t="n"/>
+      <c r="I54" s="119" t="n"/>
+      <c r="J54" s="118" t="n"/>
+      <c r="K54" s="120" t="n"/>
+      <c r="L54" s="107" t="n"/>
+      <c r="M54" s="108" t="n"/>
+      <c r="N54" s="114" t="n"/>
+      <c r="O54" s="101" t="n"/>
+      <c r="P54" s="101" t="n"/>
+      <c r="Q54" s="101" t="n"/>
+      <c r="R54" s="101" t="n"/>
+      <c r="S54" s="101" t="n"/>
     </row>
     <row r="55" ht="15" customHeight="1">
-      <c r="A55" s="13" t="n"/>
-      <c r="B55" s="14" t="n"/>
-      <c r="C55" s="36" t="n"/>
-      <c r="D55" s="30" t="n"/>
-      <c r="E55" s="14" t="n"/>
-      <c r="F55" s="15" t="n"/>
-      <c r="G55" s="25" t="n"/>
-      <c r="H55" s="26" t="n"/>
-      <c r="I55" s="61" t="n"/>
-      <c r="J55" s="62" t="n"/>
-      <c r="K55" s="63" t="n"/>
-      <c r="L55" s="63" t="n"/>
-      <c r="M55" s="63" t="n"/>
-      <c r="N55" s="81" t="n"/>
+      <c r="A55" s="115" t="n"/>
+      <c r="B55" s="115" t="n"/>
+      <c r="C55" s="116" t="n"/>
+      <c r="D55" s="115" t="n"/>
+      <c r="E55" s="115" t="n"/>
+      <c r="F55" s="117" t="n"/>
+      <c r="G55" s="118" t="n"/>
+      <c r="H55" s="118" t="n"/>
+      <c r="I55" s="119" t="n"/>
+      <c r="J55" s="118" t="n"/>
+      <c r="K55" s="120" t="n"/>
+      <c r="L55" s="107" t="n"/>
+      <c r="M55" s="108" t="n"/>
+      <c r="N55" s="114" t="n"/>
+      <c r="O55" s="101" t="n"/>
+      <c r="P55" s="101" t="n"/>
+      <c r="Q55" s="101" t="n"/>
+      <c r="R55" s="101" t="n"/>
+      <c r="S55" s="101" t="n"/>
     </row>
     <row r="56" ht="15" customHeight="1">
-      <c r="A56" s="13" t="n"/>
-      <c r="B56" s="14" t="n"/>
-      <c r="C56" s="36" t="n"/>
-      <c r="D56" s="30" t="n"/>
-      <c r="E56" s="14" t="n"/>
-      <c r="F56" s="15" t="n"/>
-      <c r="G56" s="25" t="n"/>
-      <c r="H56" s="26" t="n"/>
-      <c r="I56" s="61" t="n"/>
-      <c r="J56" s="62" t="n"/>
-      <c r="K56" s="63" t="n"/>
-      <c r="L56" s="63" t="n"/>
-      <c r="M56" s="63" t="n"/>
-      <c r="N56" s="81" t="n"/>
+      <c r="A56" s="115" t="n"/>
+      <c r="B56" s="115" t="n"/>
+      <c r="C56" s="116" t="n"/>
+      <c r="D56" s="115" t="n"/>
+      <c r="E56" s="115" t="n"/>
+      <c r="F56" s="117" t="n"/>
+      <c r="G56" s="118" t="n"/>
+      <c r="H56" s="118" t="n"/>
+      <c r="I56" s="119" t="n"/>
+      <c r="J56" s="118" t="n"/>
+      <c r="K56" s="120" t="n"/>
+      <c r="L56" s="107" t="n"/>
+      <c r="M56" s="108" t="n"/>
+      <c r="N56" s="114" t="n"/>
+      <c r="O56" s="101" t="n"/>
+      <c r="P56" s="101" t="n"/>
+      <c r="Q56" s="101" t="n"/>
+      <c r="R56" s="101" t="n"/>
+      <c r="S56" s="101" t="n"/>
     </row>
     <row r="57" ht="15" customHeight="1">
-      <c r="A57" s="13" t="n"/>
-      <c r="B57" s="14" t="n"/>
-      <c r="C57" s="36" t="n"/>
-      <c r="D57" s="30" t="n"/>
-      <c r="E57" s="14" t="n"/>
-      <c r="F57" s="15" t="n"/>
-      <c r="G57" s="25" t="n"/>
-      <c r="H57" s="26" t="n"/>
-      <c r="I57" s="61" t="n"/>
-      <c r="J57" s="62" t="n"/>
-      <c r="K57" s="63" t="n"/>
-      <c r="L57" s="63" t="n"/>
-      <c r="M57" s="63" t="n"/>
-      <c r="N57" s="81" t="n"/>
+      <c r="A57" s="115" t="n"/>
+      <c r="B57" s="115" t="n"/>
+      <c r="C57" s="116" t="n"/>
+      <c r="D57" s="115" t="n"/>
+      <c r="E57" s="115" t="n"/>
+      <c r="F57" s="117" t="n"/>
+      <c r="G57" s="118" t="n"/>
+      <c r="H57" s="118" t="n"/>
+      <c r="I57" s="119" t="n"/>
+      <c r="J57" s="118" t="n"/>
+      <c r="K57" s="120" t="n"/>
+      <c r="L57" s="107" t="n"/>
+      <c r="M57" s="108" t="n"/>
+      <c r="N57" s="114" t="n"/>
+      <c r="O57" s="101" t="n"/>
+      <c r="P57" s="101" t="n"/>
+      <c r="Q57" s="101" t="n"/>
+      <c r="R57" s="101" t="n"/>
+      <c r="S57" s="101" t="n"/>
     </row>
     <row r="58" ht="15" customHeight="1">
-      <c r="A58" s="13" t="n"/>
-      <c r="B58" s="14" t="n"/>
-      <c r="C58" s="36" t="n"/>
-      <c r="D58" s="30" t="n"/>
-      <c r="E58" s="14" t="n"/>
-      <c r="F58" s="15" t="n"/>
-      <c r="G58" s="25" t="n"/>
-      <c r="H58" s="26" t="n"/>
-      <c r="I58" s="61" t="n"/>
-      <c r="J58" s="62" t="n"/>
-      <c r="K58" s="63" t="n"/>
-      <c r="L58" s="63" t="n"/>
-      <c r="M58" s="63" t="n"/>
-      <c r="N58" s="81" t="n"/>
+      <c r="A58" s="115" t="n"/>
+      <c r="B58" s="115" t="n"/>
+      <c r="C58" s="116" t="n"/>
+      <c r="D58" s="115" t="n"/>
+      <c r="E58" s="115" t="n"/>
+      <c r="F58" s="117" t="n"/>
+      <c r="G58" s="118" t="n"/>
+      <c r="H58" s="118" t="n"/>
+      <c r="I58" s="119" t="n"/>
+      <c r="J58" s="118" t="n"/>
+      <c r="K58" s="120" t="n"/>
+      <c r="L58" s="107" t="n"/>
+      <c r="M58" s="108" t="n"/>
+      <c r="N58" s="114" t="n"/>
+      <c r="O58" s="101" t="n"/>
+      <c r="P58" s="101" t="n"/>
+      <c r="Q58" s="101" t="n"/>
+      <c r="R58" s="101" t="n"/>
+      <c r="S58" s="101" t="n"/>
     </row>
     <row r="59" ht="15" customHeight="1">
-      <c r="A59" s="13" t="n"/>
-      <c r="B59" s="14" t="n"/>
-      <c r="C59" s="36" t="n"/>
-      <c r="D59" s="30" t="n"/>
-      <c r="E59" s="14" t="n"/>
-      <c r="F59" s="15" t="n"/>
-      <c r="G59" s="25" t="n"/>
-      <c r="H59" s="26" t="n"/>
-      <c r="I59" s="61" t="n"/>
-      <c r="J59" s="62" t="n"/>
-      <c r="K59" s="63" t="n"/>
-      <c r="L59" s="63" t="n"/>
-      <c r="M59" s="63" t="n"/>
-      <c r="N59" s="81" t="n"/>
+      <c r="A59" s="115" t="n"/>
+      <c r="B59" s="115" t="n"/>
+      <c r="C59" s="116" t="n"/>
+      <c r="D59" s="115" t="n"/>
+      <c r="E59" s="115" t="n"/>
+      <c r="F59" s="117" t="n"/>
+      <c r="G59" s="118" t="n"/>
+      <c r="H59" s="118" t="n"/>
+      <c r="I59" s="119" t="n"/>
+      <c r="J59" s="118" t="n"/>
+      <c r="K59" s="120" t="n"/>
+      <c r="L59" s="107" t="n"/>
+      <c r="M59" s="108" t="n"/>
+      <c r="N59" s="114" t="n"/>
+      <c r="O59" s="101" t="n"/>
+      <c r="P59" s="101" t="n"/>
+      <c r="Q59" s="101" t="n"/>
+      <c r="R59" s="101" t="n"/>
+      <c r="S59" s="101" t="n"/>
     </row>
     <row r="60" ht="15" customHeight="1">
-      <c r="A60" s="13" t="n"/>
-      <c r="B60" s="14" t="n"/>
-      <c r="C60" s="36" t="n"/>
-      <c r="D60" s="30" t="n"/>
-      <c r="E60" s="14" t="n"/>
-      <c r="F60" s="15" t="n"/>
-      <c r="G60" s="25" t="n"/>
-      <c r="H60" s="26" t="n"/>
-      <c r="I60" s="61" t="n"/>
-      <c r="J60" s="62" t="n"/>
-      <c r="K60" s="63" t="n"/>
-      <c r="L60" s="63" t="n"/>
-      <c r="M60" s="63" t="n"/>
-      <c r="N60" s="81" t="n"/>
+      <c r="A60" s="115" t="n"/>
+      <c r="B60" s="115" t="n"/>
+      <c r="C60" s="116" t="n"/>
+      <c r="D60" s="115" t="n"/>
+      <c r="E60" s="115" t="n"/>
+      <c r="F60" s="117" t="n"/>
+      <c r="G60" s="118" t="n"/>
+      <c r="H60" s="118" t="n"/>
+      <c r="I60" s="119" t="n"/>
+      <c r="J60" s="118" t="n"/>
+      <c r="K60" s="120" t="n"/>
+      <c r="L60" s="107" t="n"/>
+      <c r="M60" s="108" t="n"/>
+      <c r="N60" s="114" t="n"/>
+      <c r="O60" s="101" t="n"/>
+      <c r="P60" s="101" t="n"/>
+      <c r="Q60" s="101" t="n"/>
+      <c r="R60" s="101" t="n"/>
+      <c r="S60" s="101" t="n"/>
     </row>
     <row r="61" ht="15" customHeight="1">
-      <c r="A61" s="13" t="n"/>
-      <c r="B61" s="14" t="n"/>
-      <c r="C61" s="36" t="n"/>
-      <c r="D61" s="30" t="n"/>
-      <c r="E61" s="14" t="n"/>
-      <c r="F61" s="15" t="n"/>
-      <c r="G61" s="25" t="n"/>
-      <c r="H61" s="26" t="n"/>
-      <c r="I61" s="61" t="n"/>
-      <c r="J61" s="62" t="n"/>
-      <c r="K61" s="63" t="n"/>
-      <c r="L61" s="63" t="n"/>
-      <c r="M61" s="63" t="n"/>
-      <c r="N61" s="81" t="n"/>
+      <c r="A61" s="115" t="n"/>
+      <c r="B61" s="115" t="n"/>
+      <c r="C61" s="116" t="n"/>
+      <c r="D61" s="115" t="n"/>
+      <c r="E61" s="115" t="n"/>
+      <c r="F61" s="117" t="n"/>
+      <c r="G61" s="118" t="n"/>
+      <c r="H61" s="118" t="n"/>
+      <c r="I61" s="119" t="n"/>
+      <c r="J61" s="118" t="n"/>
+      <c r="K61" s="120" t="n"/>
+      <c r="L61" s="107" t="n"/>
+      <c r="M61" s="108" t="n"/>
+      <c r="N61" s="114" t="n"/>
+      <c r="O61" s="101" t="n"/>
+      <c r="P61" s="101" t="n"/>
+      <c r="Q61" s="101" t="n"/>
+      <c r="R61" s="101" t="n"/>
+      <c r="S61" s="101" t="n"/>
     </row>
     <row r="62" ht="15" customHeight="1">
-      <c r="A62" s="13" t="n"/>
-      <c r="B62" s="14" t="n"/>
-      <c r="C62" s="36" t="n"/>
-      <c r="D62" s="30" t="n"/>
-      <c r="E62" s="14" t="n"/>
-      <c r="F62" s="15" t="n"/>
-      <c r="G62" s="25" t="n"/>
-      <c r="H62" s="26" t="n"/>
-      <c r="I62" s="61" t="n"/>
-      <c r="J62" s="62" t="n"/>
-      <c r="K62" s="63" t="n"/>
-      <c r="L62" s="63" t="n"/>
-      <c r="M62" s="63" t="n"/>
-      <c r="N62" s="81" t="n"/>
+      <c r="A62" s="115" t="n"/>
+      <c r="B62" s="115" t="n"/>
+      <c r="C62" s="116" t="n"/>
+      <c r="D62" s="115" t="n"/>
+      <c r="E62" s="115" t="n"/>
+      <c r="F62" s="117" t="n"/>
+      <c r="G62" s="118" t="n"/>
+      <c r="H62" s="118" t="n"/>
+      <c r="I62" s="119" t="n"/>
+      <c r="J62" s="118" t="n"/>
+      <c r="K62" s="120" t="n"/>
+      <c r="L62" s="107" t="n"/>
+      <c r="M62" s="108" t="n"/>
+      <c r="N62" s="114" t="n"/>
+      <c r="O62" s="101" t="n"/>
+      <c r="P62" s="101" t="n"/>
+      <c r="Q62" s="101" t="n"/>
+      <c r="R62" s="101" t="n"/>
+      <c r="S62" s="101" t="n"/>
     </row>
     <row r="63" ht="15" customHeight="1">
-      <c r="A63" s="13" t="n"/>
-      <c r="B63" s="14" t="n"/>
-      <c r="C63" s="36" t="n"/>
-      <c r="D63" s="30" t="n"/>
-      <c r="E63" s="14" t="n"/>
-      <c r="F63" s="15" t="n"/>
-      <c r="G63" s="25" t="n"/>
-      <c r="H63" s="26" t="n"/>
-      <c r="I63" s="61" t="n"/>
-      <c r="J63" s="62" t="n"/>
-      <c r="K63" s="63" t="n"/>
-      <c r="L63" s="63" t="n"/>
-      <c r="M63" s="63" t="n"/>
-      <c r="N63" s="81" t="n"/>
+      <c r="A63" s="115" t="n"/>
+      <c r="B63" s="115" t="n"/>
+      <c r="C63" s="116" t="n"/>
+      <c r="D63" s="115" t="n"/>
+      <c r="E63" s="115" t="n"/>
+      <c r="F63" s="117" t="n"/>
+      <c r="G63" s="118" t="n"/>
+      <c r="H63" s="118" t="n"/>
+      <c r="I63" s="119" t="n"/>
+      <c r="J63" s="118" t="n"/>
+      <c r="K63" s="120" t="n"/>
+      <c r="L63" s="107" t="n"/>
+      <c r="M63" s="108" t="n"/>
+      <c r="N63" s="114" t="n"/>
+      <c r="O63" s="101" t="n"/>
+      <c r="P63" s="101" t="n"/>
+      <c r="Q63" s="101" t="n"/>
+      <c r="R63" s="101" t="n"/>
+      <c r="S63" s="101" t="n"/>
     </row>
     <row r="64" ht="15" customHeight="1">
-      <c r="A64" s="13" t="n"/>
-      <c r="B64" s="14" t="n"/>
-      <c r="C64" s="36" t="n"/>
-      <c r="D64" s="30" t="n"/>
-      <c r="E64" s="14" t="n"/>
-      <c r="F64" s="15" t="n"/>
-      <c r="G64" s="25" t="n"/>
-      <c r="H64" s="26" t="n"/>
-      <c r="I64" s="61" t="n"/>
-      <c r="J64" s="62" t="n"/>
-      <c r="K64" s="63" t="n"/>
-      <c r="L64" s="63" t="n"/>
-      <c r="M64" s="63" t="n"/>
-      <c r="N64" s="81" t="n"/>
+      <c r="A64" s="115" t="n"/>
+      <c r="B64" s="115" t="n"/>
+      <c r="C64" s="116" t="n"/>
+      <c r="D64" s="115" t="n"/>
+      <c r="E64" s="115" t="n"/>
+      <c r="F64" s="117" t="n"/>
+      <c r="G64" s="118" t="n"/>
+      <c r="H64" s="118" t="n"/>
+      <c r="I64" s="119" t="n"/>
+      <c r="J64" s="118" t="n"/>
+      <c r="K64" s="120" t="n"/>
+      <c r="L64" s="107" t="n"/>
+      <c r="M64" s="108" t="n"/>
+      <c r="N64" s="114" t="n"/>
+      <c r="O64" s="101" t="n"/>
+      <c r="P64" s="101" t="n"/>
+      <c r="Q64" s="101" t="n"/>
+      <c r="R64" s="101" t="n"/>
+      <c r="S64" s="101" t="n"/>
     </row>
     <row r="65" ht="15" customHeight="1">
-      <c r="A65" s="13" t="n"/>
-      <c r="B65" s="14" t="n"/>
-      <c r="C65" s="36" t="n"/>
-      <c r="D65" s="30" t="n"/>
-      <c r="E65" s="14" t="n"/>
-      <c r="F65" s="15" t="n"/>
-      <c r="G65" s="25" t="n"/>
-      <c r="H65" s="26" t="n"/>
-      <c r="I65" s="61" t="n"/>
-      <c r="J65" s="62" t="n"/>
-      <c r="K65" s="63" t="n"/>
-      <c r="L65" s="63" t="n"/>
-      <c r="M65" s="63" t="n"/>
-      <c r="N65" s="81" t="n"/>
+      <c r="A65" s="115" t="n"/>
+      <c r="B65" s="115" t="n"/>
+      <c r="C65" s="116" t="n"/>
+      <c r="D65" s="115" t="n"/>
+      <c r="E65" s="115" t="n"/>
+      <c r="F65" s="117" t="n"/>
+      <c r="G65" s="118" t="n"/>
+      <c r="H65" s="118" t="n"/>
+      <c r="I65" s="119" t="n"/>
+      <c r="J65" s="118" t="n"/>
+      <c r="K65" s="120" t="n"/>
+      <c r="L65" s="107" t="n"/>
+      <c r="M65" s="108" t="n"/>
+      <c r="N65" s="114" t="n"/>
+      <c r="O65" s="101" t="n"/>
+      <c r="P65" s="101" t="n"/>
+      <c r="Q65" s="101" t="n"/>
+      <c r="R65" s="101" t="n"/>
+      <c r="S65" s="101" t="n"/>
     </row>
     <row r="66" ht="15" customHeight="1">
-      <c r="A66" s="13" t="n"/>
-      <c r="B66" s="14" t="n"/>
-      <c r="C66" s="36" t="n"/>
-      <c r="D66" s="30" t="n"/>
-      <c r="E66" s="14" t="n"/>
-      <c r="F66" s="15" t="n"/>
-      <c r="G66" s="25" t="n"/>
-      <c r="H66" s="26" t="n"/>
-      <c r="I66" s="61" t="n"/>
-      <c r="J66" s="62" t="n"/>
-      <c r="K66" s="63" t="n"/>
-      <c r="L66" s="63" t="n"/>
-      <c r="M66" s="63" t="n"/>
-      <c r="N66" s="81" t="n"/>
+      <c r="A66" s="115" t="n"/>
+      <c r="B66" s="115" t="n"/>
+      <c r="C66" s="116" t="n"/>
+      <c r="D66" s="115" t="n"/>
+      <c r="E66" s="115" t="n"/>
+      <c r="F66" s="117" t="n"/>
+      <c r="G66" s="118" t="n"/>
+      <c r="H66" s="118" t="n"/>
+      <c r="I66" s="119" t="n"/>
+      <c r="J66" s="118" t="n"/>
+      <c r="K66" s="120" t="n"/>
+      <c r="L66" s="107" t="n"/>
+      <c r="M66" s="108" t="n"/>
+      <c r="N66" s="114" t="n"/>
+      <c r="O66" s="101" t="n"/>
+      <c r="P66" s="101" t="n"/>
+      <c r="Q66" s="101" t="n"/>
+      <c r="R66" s="101" t="n"/>
+      <c r="S66" s="101" t="n"/>
     </row>
     <row r="67" ht="15" customHeight="1">
-      <c r="A67" s="13" t="n"/>
-      <c r="B67" s="14" t="n"/>
-      <c r="C67" s="36" t="n"/>
-      <c r="D67" s="30" t="n"/>
-      <c r="E67" s="14" t="n"/>
-      <c r="F67" s="15" t="n"/>
-      <c r="G67" s="25" t="n"/>
-      <c r="H67" s="26" t="n"/>
-      <c r="I67" s="61" t="n"/>
-      <c r="J67" s="62" t="n"/>
-      <c r="K67" s="63" t="n"/>
-      <c r="L67" s="63" t="n"/>
-      <c r="M67" s="63" t="n"/>
-      <c r="N67" s="81" t="n"/>
+      <c r="A67" s="115" t="n"/>
+      <c r="B67" s="115" t="n"/>
+      <c r="C67" s="116" t="n"/>
+      <c r="D67" s="115" t="n"/>
+      <c r="E67" s="115" t="n"/>
+      <c r="F67" s="117" t="n"/>
+      <c r="G67" s="118" t="n"/>
+      <c r="H67" s="118" t="n"/>
+      <c r="I67" s="119" t="n"/>
+      <c r="J67" s="118" t="n"/>
+      <c r="K67" s="120" t="n"/>
+      <c r="L67" s="107" t="n"/>
+      <c r="M67" s="108" t="n"/>
+      <c r="N67" s="114" t="n"/>
+      <c r="O67" s="101" t="n"/>
+      <c r="P67" s="101" t="n"/>
+      <c r="Q67" s="101" t="n"/>
+      <c r="R67" s="101" t="n"/>
+      <c r="S67" s="101" t="n"/>
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="A68" s="13" t="n"/>
@@ -2924,24 +3426,72 @@
       <c r="N75" s="81" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="66">
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K47:M47"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K44:M44"/>
     <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K40:M40"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K31:M31"/>
     <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K67:M67"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K56:M56"/>
     <mergeCell ref="A16:F18"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="K59:M59"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K27:M27"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K53:M53"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="K37:M37"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K49:M49"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K24:M24"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K55:M55"/>
+    <mergeCell ref="K35:M35"/>
     <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="K29:M29"/>
     <mergeCell ref="I9:J9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>